<commit_message>
end of collecting data chapter
</commit_message>
<xml_diff>
--- a/inst/data/messy_ktc_data.xlsx
+++ b/inst/data/messy_ktc_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="150">
   <si>
     <t>Trench</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>Mollusc data</t>
+  </si>
+  <si>
+    <t>= contains complete vessels</t>
   </si>
 </sst>
 </file>
@@ -478,12 +481,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -498,12 +507,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,7 +819,7 @@
   <dimension ref="A1:X217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +933,7 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>14</v>
       </c>
       <c r="G3">
@@ -1512,7 +1523,7 @@
       <c r="E13">
         <v>2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>51</v>
       </c>
       <c r="G13">
@@ -1670,6 +1681,10 @@
       </c>
       <c r="I16" s="1">
         <v>39657</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>